<commit_message>
test data's document create function.
</commit_message>
<xml_diff>
--- a/AuroraSelenium/resources/TestCase_Template.xlsx
+++ b/AuroraSelenium/resources/TestCase_Template.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="90" windowWidth="20475" windowHeight="9855"/>
+    <workbookView xWindow="5620" yWindow="900" windowWidth="20480" windowHeight="9860"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TestCase" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>TestSuite</t>
     <phoneticPr fontId="1"/>
@@ -41,6 +44,14 @@
     <t>Screenshot</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Value</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -50,14 +61,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -127,7 +138,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -159,7 +170,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -170,7 +181,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -471,306 +482,373 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6">
       <c r="A5" s="4">
         <f>ROW()-4</f>
         <v>1</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="4">
         <f t="shared" ref="A6:A69" si="0">ROW()-4</f>
         <v>2</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="4">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="4">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="4">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="4">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="4">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="4">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="4">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="4">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="4">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="4">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="4">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
-      <c r="D32" s="5"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="4">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="4">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -778,8 +856,10 @@
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="4">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -787,8 +867,10 @@
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="4">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -796,8 +878,10 @@
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="4">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -805,8 +889,10 @@
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="4">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -814,8 +900,10 @@
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="4">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -823,8 +911,10 @@
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="4">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -832,8 +922,10 @@
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="4">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -841,8 +933,10 @@
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="4">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -850,8 +944,10 @@
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="4">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -859,8 +955,10 @@
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="4">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -868,8 +966,10 @@
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="4">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -877,8 +977,10 @@
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="4">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -886,8 +988,10 @@
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="4">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -895,8 +999,10 @@
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="4">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -904,8 +1010,10 @@
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="4">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -913,8 +1021,10 @@
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="4">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -922,8 +1032,10 @@
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="4">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -931,8 +1043,10 @@
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="4">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -940,8 +1054,10 @@
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="4">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -949,8 +1065,10 @@
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" s="4">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -958,8 +1076,10 @@
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" s="4">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -967,8 +1087,10 @@
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" s="4">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -976,8 +1098,10 @@
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" s="4">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -985,8 +1109,10 @@
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" s="4">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -994,8 +1120,10 @@
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" s="4">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -1003,8 +1131,10 @@
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" s="4">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -1012,8 +1142,10 @@
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" s="4">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -1021,8 +1153,10 @@
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" s="4">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -1030,8 +1164,10 @@
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" s="4">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -1039,8 +1175,10 @@
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" s="4">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -1048,8 +1186,10 @@
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" s="4">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -1057,8 +1197,10 @@
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" s="4">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -1066,8 +1208,10 @@
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" s="4">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -1075,8 +1219,10 @@
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" s="4">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -1084,8 +1230,10 @@
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" s="4">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -1093,18 +1241,20 @@
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="D5:D10">
-    <cfRule type="cellIs" dxfId="3" priority="15" operator="equal">
+  <conditionalFormatting sqref="F5:F10">
+    <cfRule type="cellIs" dxfId="3" priority="13" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="15" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="13" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11:D33">
+  <conditionalFormatting sqref="F11:F33">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -1113,39 +1263,18 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D6:D33">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F6:F33">
       <formula1>"No,Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5">
       <formula1>"No,Yes"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>